<commit_message>
Mensajes emergentes en objetos esperados y reales
</commit_message>
<xml_diff>
--- a/Locale/Locale.xlsx
+++ b/Locale/Locale.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="205">
   <si>
     <t xml:space="preserve">Delete character data</t>
   </si>
@@ -157,16 +157,28 @@
     <t xml:space="preserve">Objetos</t>
   </si>
   <si>
+    <t xml:space="preserve">Dusts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polvos</t>
+  </si>
+  <si>
     <t xml:space="preserve">Essences</t>
   </si>
   <si>
     <t xml:space="preserve">Esencias</t>
   </si>
   <si>
-    <t xml:space="preserve">Dusts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Polvos</t>
+    <t xml:space="preserve">Shards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fragmentos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crystals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cristales</t>
   </si>
   <si>
     <t xml:space="preserve">Update database</t>
@@ -193,6 +205,24 @@
     <t xml:space="preserve">Purgar base de datos</t>
   </si>
   <si>
+    <t xml:space="preserve">Starting auto disenchant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iniciando el desencantado automático</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cancelling auto disenchant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cancelando el desencantado automático</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enchanting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encantamiento</t>
+  </si>
+  <si>
     <t xml:space="preserve">Initialized</t>
   </si>
   <si>
@@ -292,105 +322,192 @@
     <t xml:space="preserve">Sólo desencanta estas calidades de objeto.</t>
   </si>
   <si>
-    <t xml:space="preserve">Remove from session ignore list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eliminar de la lista de ignorados de la sesión</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Are you sure you want to remove this ignored item?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">¿Está seguro de que desea eliminar este elemento ignorado?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remove from permanent ignore list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eliminar de la lista permanente de ignorados</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clear</t>
+    <t xml:space="preserve">Clean session</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Limpiar sesión</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clear the ignore list of this session.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Limpiar lista de ignorados de esta sesión.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clean permanent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Limpiar permanente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clear the permanent ignore list.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Limpiar la lista de ignorados permanentemente.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uncommon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poco Común</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disable all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desactivar todo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disable all settings.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desactiva todos los ajustes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tooltips</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mensajes emergentes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable tooltips about enchanting materials.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activar información sobre materiales de encantamiento.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Press key to show</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pulse la tecla para mostrar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mostrar título</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toggle showing title.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Habilita mostrar el título.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show ItemID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mostrar ItemID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toggle showing item ids.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Habilita mostrar el ID de objetos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show zero values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mostrar valores con cero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toggle showing zero values.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Habilita mostrar valores cero.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Items to show</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elementos para mostrar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Items to show in tooltip.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elementos a mostrar en el mensaje emergente.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show expected essences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mostrar esencias esperadas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toggle showing of expected essences on items.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Habilita mostrar esencias esperadas en objetos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show real essences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mostrar esencias reales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toggle showing of real essences on items.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Habilita mostrar esencias reales de objetos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Base de datos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actualizar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update database manually.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actualizar base de datos manualmente.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consolidate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consolidar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consolidate players and items in database.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consolidar jugadores y objetos en la base de datos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are you sure you want to consolidate the database?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Estás seguro de que quieres consolidar la base de datos entera?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clean up</t>
   </si>
   <si>
     <t xml:space="preserve">Limpiar</t>
   </si>
   <si>
-    <t xml:space="preserve">Clear the ignore list of this session.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Limpiar lista de ignorados de esta sesión.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uncommon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Poco Común</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rare</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Raro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Epic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Epico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tooltips</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mensajes emergentes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enable tooltips about enchanting materials.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Activar información sobre materiales de encantamiento.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Base de datos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Update</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actualizar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Update database manually.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actualizar base de datos manualmente.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consolidate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consolidar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consolidate players and items in database.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consolidar jugadores y objetos en la base de datos.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Are you sure you want to consolidate the database?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">¿Estás seguro de que quieres consolidar la base de datos entera?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clean up</t>
-  </si>
-  <si>
     <t xml:space="preserve">Clean up all database by removing old data.</t>
   </si>
   <si>
@@ -451,6 +568,24 @@
     <t xml:space="preserve">Desencantado automático</t>
   </si>
   <si>
+    <t xml:space="preserve">Items left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Objetos restantes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opens settings window.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abre la ventana de configuración.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Settings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuración</t>
+  </si>
+  <si>
     <t xml:space="preserve">Do not disenchant this item during this game session.</t>
   </si>
   <si>
@@ -472,10 +607,10 @@
     <t xml:space="preserve">Sí</t>
   </si>
   <si>
-    <t xml:space="preserve">Add this item to the ignore list.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Añade este elemento a la lista de ignorados.</t>
+    <t xml:space="preserve">Add this item to the permanent ignore list.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Añade este elemento a la lista de ignorados permanente.</t>
   </si>
   <si>
     <t xml:space="preserve">Ignore</t>
@@ -484,18 +619,6 @@
     <t xml:space="preserve">Ignorar</t>
   </si>
   <si>
-    <t xml:space="preserve">Close window</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cerrar ventana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Close</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cerrar</t>
-  </si>
-  <si>
     <t xml:space="preserve">You don't have enough skill level.</t>
   </si>
   <si>
@@ -512,12 +635,6 @@
   </si>
   <si>
     <t xml:space="preserve">Plugins principales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Settings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Configuración</t>
   </si>
 </sst>
 </file>
@@ -1138,11 +1255,11 @@
       </c>
       <c r="C25" s="1" t="str">
         <f aca="false">IF(A25="", "", "L["""&amp;A25&amp;"""] = true")</f>
-        <v>L["Essences"] = true</v>
+        <v>L["Dusts"] = true</v>
       </c>
       <c r="D25" s="1" t="str">
         <f aca="false">IF(A25="", "", "L["""&amp;A25&amp;"""] = """ &amp; B25 &amp; """")</f>
-        <v>L["Essences"] = "Esencias"</v>
+        <v>L["Dusts"] = "Polvos"</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1154,11 +1271,11 @@
       </c>
       <c r="C26" s="1" t="str">
         <f aca="false">IF(A26="", "", "L["""&amp;A26&amp;"""] = true")</f>
-        <v>L["Dusts"] = true</v>
+        <v>L["Essences"] = true</v>
       </c>
       <c r="D26" s="1" t="str">
         <f aca="false">IF(A26="", "", "L["""&amp;A26&amp;"""] = """ &amp; B26 &amp; """")</f>
-        <v>L["Dusts"] = "Polvos"</v>
+        <v>L["Essences"] = "Esencias"</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1170,11 +1287,11 @@
       </c>
       <c r="C27" s="1" t="str">
         <f aca="false">IF(A27="", "", "L["""&amp;A27&amp;"""] = true")</f>
-        <v>L["Update database"] = true</v>
+        <v>L["Shards"] = true</v>
       </c>
       <c r="D27" s="1" t="str">
         <f aca="false">IF(A27="", "", "L["""&amp;A27&amp;"""] = """ &amp; B27 &amp; """")</f>
-        <v>L["Update database"] = "Actualizar base de datos"</v>
+        <v>L["Shards"] = "Fragmentos"</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1186,11 +1303,11 @@
       </c>
       <c r="C28" s="1" t="str">
         <f aca="false">IF(A28="", "", "L["""&amp;A28&amp;"""] = true")</f>
-        <v>L["Consolidate database"] = true</v>
+        <v>L["Crystals"] = true</v>
       </c>
       <c r="D28" s="1" t="str">
         <f aca="false">IF(A28="", "", "L["""&amp;A28&amp;"""] = """ &amp; B28 &amp; """")</f>
-        <v>L["Consolidate database"] = "Consolidar la base de datos"</v>
+        <v>L["Crystals"] = "Cristales"</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1202,11 +1319,11 @@
       </c>
       <c r="C29" s="1" t="str">
         <f aca="false">IF(A29="", "", "L["""&amp;A29&amp;"""] = true")</f>
-        <v>L["Clean database"] = true</v>
+        <v>L["Update database"] = true</v>
       </c>
       <c r="D29" s="1" t="str">
         <f aca="false">IF(A29="", "", "L["""&amp;A29&amp;"""] = """ &amp; B29 &amp; """")</f>
-        <v>L["Clean database"] = "Limpiar la base de datos"</v>
+        <v>L["Update database"] = "Actualizar base de datos"</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1218,11 +1335,11 @@
       </c>
       <c r="C30" s="1" t="str">
         <f aca="false">IF(A30="", "", "L["""&amp;A30&amp;"""] = true")</f>
-        <v>L["Purge database"] = true</v>
+        <v>L["Consolidate database"] = true</v>
       </c>
       <c r="D30" s="1" t="str">
         <f aca="false">IF(A30="", "", "L["""&amp;A30&amp;"""] = """ &amp; B30 &amp; """")</f>
-        <v>L["Purge database"] = "Purgar base de datos"</v>
+        <v>L["Consolidate database"] = "Consolidar la base de datos"</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1234,11 +1351,11 @@
       </c>
       <c r="C31" s="1" t="str">
         <f aca="false">IF(A31="", "", "L["""&amp;A31&amp;"""] = true")</f>
-        <v>L["Initialized"] = true</v>
+        <v>L["Clean database"] = true</v>
       </c>
       <c r="D31" s="1" t="str">
         <f aca="false">IF(A31="", "", "L["""&amp;A31&amp;"""] = """ &amp; B31 &amp; """")</f>
-        <v>L["Initialized"] = "Inicializado"</v>
+        <v>L["Clean database"] = "Limpiar la base de datos"</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1250,11 +1367,11 @@
       </c>
       <c r="C32" s="1" t="str">
         <f aca="false">IF(A32="", "", "L["""&amp;A32&amp;"""] = true")</f>
-        <v>L["Left Click"] = true</v>
+        <v>L["Purge database"] = true</v>
       </c>
       <c r="D32" s="1" t="str">
         <f aca="false">IF(A32="", "", "L["""&amp;A32&amp;"""] = """ &amp; B32 &amp; """")</f>
-        <v>L["Left Click"] = "Clic Izquierdo"</v>
+        <v>L["Purge database"] = "Purgar base de datos"</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1266,11 +1383,11 @@
       </c>
       <c r="C33" s="1" t="str">
         <f aca="false">IF(A33="", "", "L["""&amp;A33&amp;"""] = true")</f>
-        <v>L["Open main window"] = true</v>
+        <v>L["Starting auto disenchant"] = true</v>
       </c>
       <c r="D33" s="1" t="str">
         <f aca="false">IF(A33="", "", "L["""&amp;A33&amp;"""] = """ &amp; B33 &amp; """")</f>
-        <v>L["Open main window"] = "Abrir la ventana principal"</v>
+        <v>L["Starting auto disenchant"] = "Iniciando el desencantado automático"</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1282,11 +1399,11 @@
       </c>
       <c r="C34" s="1" t="str">
         <f aca="false">IF(A34="", "", "L["""&amp;A34&amp;"""] = true")</f>
-        <v>L["Right Click"] = true</v>
+        <v>L["Cancelling auto disenchant"] = true</v>
       </c>
       <c r="D34" s="1" t="str">
         <f aca="false">IF(A34="", "", "L["""&amp;A34&amp;"""] = """ &amp; B34 &amp; """")</f>
-        <v>L["Right Click"] = "Clic Derecho"</v>
+        <v>L["Cancelling auto disenchant"] = "Cancelando el desencantado automático"</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1298,11 +1415,11 @@
       </c>
       <c r="C35" s="1" t="str">
         <f aca="false">IF(A35="", "", "L["""&amp;A35&amp;"""] = true")</f>
-        <v>L["Open settings window"] = true</v>
+        <v>L["Enchanting"] = true</v>
       </c>
       <c r="D35" s="1" t="str">
         <f aca="false">IF(A35="", "", "L["""&amp;A35&amp;"""] = """ &amp; B35 &amp; """")</f>
-        <v>L["Open settings window"] = "Abrir la ventana de configuración"</v>
+        <v>L["Enchanting"] = "Encantamiento"</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1314,11 +1431,11 @@
       </c>
       <c r="C36" s="1" t="str">
         <f aca="false">IF(A36="", "", "L["""&amp;A36&amp;"""] = true")</f>
-        <v>L["Advanced"] = true</v>
+        <v>L["Initialized"] = true</v>
       </c>
       <c r="D36" s="1" t="str">
         <f aca="false">IF(A36="", "", "L["""&amp;A36&amp;"""] = """ &amp; B36 &amp; """")</f>
-        <v>L["Advanced"] = "Avanzado"</v>
+        <v>L["Initialized"] = "Inicializado"</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1330,11 +1447,11 @@
       </c>
       <c r="C37" s="1" t="str">
         <f aca="false">IF(A37="", "", "L["""&amp;A37&amp;"""] = true")</f>
-        <v>L["Enable debug"] = true</v>
+        <v>L["Left Click"] = true</v>
       </c>
       <c r="D37" s="1" t="str">
         <f aca="false">IF(A37="", "", "L["""&amp;A37&amp;"""] = """ &amp; B37 &amp; """")</f>
-        <v>L["Enable debug"] = "Habilitar depuración"</v>
+        <v>L["Left Click"] = "Clic Izquierdo"</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1342,95 +1459,95 @@
         <v>71</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C38" s="1" t="str">
         <f aca="false">IF(A38="", "", "L["""&amp;A38&amp;"""] = true")</f>
-        <v>L["General"] = true</v>
+        <v>L["Open main window"] = true</v>
       </c>
       <c r="D38" s="1" t="str">
         <f aca="false">IF(A38="", "", "L["""&amp;A38&amp;"""] = """ &amp; B38 &amp; """")</f>
-        <v>L["General"] = "General"</v>
+        <v>L["Open main window"] = "Abrir la ventana principal"</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C39" s="1" t="str">
         <f aca="false">IF(A39="", "", "L["""&amp;A39&amp;"""] = true")</f>
-        <v>L["Disenchant"] = true</v>
+        <v>L["Right Click"] = true</v>
       </c>
       <c r="D39" s="1" t="str">
         <f aca="false">IF(A39="", "", "L["""&amp;A39&amp;"""] = """ &amp; B39 &amp; """")</f>
-        <v>L["Disenchant"] = "Desencantar"</v>
+        <v>L["Right Click"] = "Clic Derecho"</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C40" s="1" t="str">
         <f aca="false">IF(A40="", "", "L["""&amp;A40&amp;"""] = true")</f>
-        <v>L["Enable"] = true</v>
+        <v>L["Open settings window"] = true</v>
       </c>
       <c r="D40" s="1" t="str">
         <f aca="false">IF(A40="", "", "L["""&amp;A40&amp;"""] = """ &amp; B40 &amp; """")</f>
-        <v>L["Enable"] = "Activar"</v>
+        <v>L["Open settings window"] = "Abrir la ventana de configuración"</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C41" s="1" t="str">
         <f aca="false">IF(A41="", "", "L["""&amp;A41&amp;"""] = true")</f>
-        <v>L["Enable auto disenchant items."] = true</v>
+        <v>L["Advanced"] = true</v>
       </c>
       <c r="D41" s="1" t="str">
         <f aca="false">IF(A41="", "", "L["""&amp;A41&amp;"""] = """ &amp; B41 &amp; """")</f>
-        <v>L["Enable auto disenchant items."] = "Activa desencantar automáticamente objetos."</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>L["Advanced"] = "Avanzado"</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C42" s="1" t="str">
         <f aca="false">IF(A42="", "", "L["""&amp;A42&amp;"""] = true")</f>
-        <v>L["Auto disenchant update time"] = true</v>
+        <v>L["Enable debug"] = true</v>
       </c>
       <c r="D42" s="1" t="str">
         <f aca="false">IF(A42="", "", "L["""&amp;A42&amp;"""] = """ &amp; B42 &amp; """")</f>
-        <v>L["Auto disenchant update time"] = "Tiempo de actualización automática del desencantado"</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>L["Enable debug"] = "Habilitar depuración"</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>81</v>
       </c>
       <c r="C43" s="1" t="str">
         <f aca="false">IF(A43="", "", "L["""&amp;A43&amp;"""] = true")</f>
-        <v>L["Sets how often the auto disenchant is executed (in seconds)."] = true</v>
+        <v>L["General"] = true</v>
       </c>
       <c r="D43" s="1" t="str">
         <f aca="false">IF(A43="", "", "L["""&amp;A43&amp;"""] = """ &amp; B43 &amp; """")</f>
-        <v>L["Sets how often the auto disenchant is executed (in seconds)."] = "Establece la frecuencia con la que se ejecuta el auto desencantado (en segundos)."</v>
+        <v>L["General"] = "General"</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1442,11 +1559,11 @@
       </c>
       <c r="C44" s="1" t="str">
         <f aca="false">IF(A44="", "", "L["""&amp;A44&amp;"""] = true")</f>
-        <v>L["Only soulbound items"] = true</v>
+        <v>L["Disenchant"] = true</v>
       </c>
       <c r="D44" s="1" t="str">
         <f aca="false">IF(A44="", "", "L["""&amp;A44&amp;"""] = """ &amp; B44 &amp; """")</f>
-        <v>L["Only soulbound items"] = "Sólo objetos ligados al alma"</v>
+        <v>L["Disenchant"] = "Desencantar"</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1458,11 +1575,11 @@
       </c>
       <c r="C45" s="1" t="str">
         <f aca="false">IF(A45="", "", "L["""&amp;A45&amp;"""] = true")</f>
-        <v>L["Enable only disenchant soulbound items."] = true</v>
+        <v>L["Enable"] = true</v>
       </c>
       <c r="D45" s="1" t="str">
         <f aca="false">IF(A45="", "", "L["""&amp;A45&amp;"""] = """ &amp; B45 &amp; """")</f>
-        <v>L["Enable only disenchant soulbound items."] = "Activar sólo desencantar objetos ligados al alma."</v>
+        <v>L["Enable"] = "Activar"</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1474,14 +1591,14 @@
       </c>
       <c r="C46" s="1" t="str">
         <f aca="false">IF(A46="", "", "L["""&amp;A46&amp;"""] = true")</f>
-        <v>L["Item qualities"] = true</v>
+        <v>L["Enable auto disenchant items."] = true</v>
       </c>
       <c r="D46" s="1" t="str">
         <f aca="false">IF(A46="", "", "L["""&amp;A46&amp;"""] = """ &amp; B46 &amp; """")</f>
-        <v>L["Item qualities"] = "Calidad del objeto"</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>L["Enable auto disenchant items."] = "Activa desencantar automáticamente objetos."</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
         <v>88</v>
       </c>
@@ -1490,14 +1607,14 @@
       </c>
       <c r="C47" s="1" t="str">
         <f aca="false">IF(A47="", "", "L["""&amp;A47&amp;"""] = true")</f>
-        <v>L["Only disenchant these item qualities."] = true</v>
+        <v>L["Auto disenchant update time"] = true</v>
       </c>
       <c r="D47" s="1" t="str">
         <f aca="false">IF(A47="", "", "L["""&amp;A47&amp;"""] = """ &amp; B47 &amp; """")</f>
-        <v>L["Only disenchant these item qualities."] = "Sólo desencanta estas calidades de objeto."</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>L["Auto disenchant update time"] = "Tiempo de actualización automática del desencantado"</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
         <v>90</v>
       </c>
@@ -1506,14 +1623,14 @@
       </c>
       <c r="C48" s="1" t="str">
         <f aca="false">IF(A48="", "", "L["""&amp;A48&amp;"""] = true")</f>
-        <v>L["Remove from session ignore list"] = true</v>
+        <v>L["Sets how often the auto disenchant is executed (in seconds)."] = true</v>
       </c>
       <c r="D48" s="1" t="str">
         <f aca="false">IF(A48="", "", "L["""&amp;A48&amp;"""] = """ &amp; B48 &amp; """")</f>
-        <v>L["Remove from session ignore list"] = "Eliminar de la lista de ignorados de la sesión"</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>L["Sets how often the auto disenchant is executed (in seconds)."] = "Establece la frecuencia con la que se ejecuta el auto desencantado (en segundos)."</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
         <v>92</v>
       </c>
@@ -1522,11 +1639,11 @@
       </c>
       <c r="C49" s="1" t="str">
         <f aca="false">IF(A49="", "", "L["""&amp;A49&amp;"""] = true")</f>
-        <v>L["Are you sure you want to remove this ignored item?"] = true</v>
+        <v>L["Only soulbound items"] = true</v>
       </c>
       <c r="D49" s="1" t="str">
         <f aca="false">IF(A49="", "", "L["""&amp;A49&amp;"""] = """ &amp; B49 &amp; """")</f>
-        <v>L["Are you sure you want to remove this ignored item?"] = "¿Está seguro de que desea eliminar este elemento ignorado?"</v>
+        <v>L["Only soulbound items"] = "Sólo objetos ligados al alma"</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1538,11 +1655,11 @@
       </c>
       <c r="C50" s="1" t="str">
         <f aca="false">IF(A50="", "", "L["""&amp;A50&amp;"""] = true")</f>
-        <v>L["Remove from permanent ignore list"] = true</v>
+        <v>L["Enable only disenchant soulbound items."] = true</v>
       </c>
       <c r="D50" s="1" t="str">
         <f aca="false">IF(A50="", "", "L["""&amp;A50&amp;"""] = """ &amp; B50 &amp; """")</f>
-        <v>L["Remove from permanent ignore list"] = "Eliminar de la lista permanente de ignorados"</v>
+        <v>L["Enable only disenchant soulbound items."] = "Activar sólo desencantar objetos ligados al alma."</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1554,11 +1671,11 @@
       </c>
       <c r="C51" s="1" t="str">
         <f aca="false">IF(A51="", "", "L["""&amp;A51&amp;"""] = true")</f>
-        <v>L["Clear"] = true</v>
+        <v>L["Item qualities"] = true</v>
       </c>
       <c r="D51" s="1" t="str">
         <f aca="false">IF(A51="", "", "L["""&amp;A51&amp;"""] = """ &amp; B51 &amp; """")</f>
-        <v>L["Clear"] = "Limpiar"</v>
+        <v>L["Item qualities"] = "Calidad del objeto"</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1570,11 +1687,11 @@
       </c>
       <c r="C52" s="1" t="str">
         <f aca="false">IF(A52="", "", "L["""&amp;A52&amp;"""] = true")</f>
-        <v>L["Clear the ignore list of this session."] = true</v>
+        <v>L["Only disenchant these item qualities."] = true</v>
       </c>
       <c r="D52" s="1" t="str">
         <f aca="false">IF(A52="", "", "L["""&amp;A52&amp;"""] = """ &amp; B52 &amp; """")</f>
-        <v>L["Clear the ignore list of this session."] = "Limpiar lista de ignorados de esta sesión."</v>
+        <v>L["Only disenchant these item qualities."] = "Sólo desencanta estas calidades de objeto."</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1586,11 +1703,11 @@
       </c>
       <c r="C53" s="1" t="str">
         <f aca="false">IF(A53="", "", "L["""&amp;A53&amp;"""] = true")</f>
-        <v>L["Uncommon"] = true</v>
+        <v>L["Clean session"] = true</v>
       </c>
       <c r="D53" s="1" t="str">
         <f aca="false">IF(A53="", "", "L["""&amp;A53&amp;"""] = """ &amp; B53 &amp; """")</f>
-        <v>L["Uncommon"] = "Poco Común"</v>
+        <v>L["Clean session"] = "Limpiar sesión"</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1602,11 +1719,11 @@
       </c>
       <c r="C54" s="1" t="str">
         <f aca="false">IF(A54="", "", "L["""&amp;A54&amp;"""] = true")</f>
-        <v>L["Rare"] = true</v>
+        <v>L["Clear the ignore list of this session."] = true</v>
       </c>
       <c r="D54" s="1" t="str">
         <f aca="false">IF(A54="", "", "L["""&amp;A54&amp;"""] = """ &amp; B54 &amp; """")</f>
-        <v>L["Rare"] = "Raro"</v>
+        <v>L["Clear the ignore list of this session."] = "Limpiar lista de ignorados de esta sesión."</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1618,11 +1735,11 @@
       </c>
       <c r="C55" s="1" t="str">
         <f aca="false">IF(A55="", "", "L["""&amp;A55&amp;"""] = true")</f>
-        <v>L["Epic"] = true</v>
+        <v>L["Clean permanent"] = true</v>
       </c>
       <c r="D55" s="1" t="str">
         <f aca="false">IF(A55="", "", "L["""&amp;A55&amp;"""] = """ &amp; B55 &amp; """")</f>
-        <v>L["Epic"] = "Epico"</v>
+        <v>L["Clean permanent"] = "Limpiar permanente"</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1634,14 +1751,14 @@
       </c>
       <c r="C56" s="1" t="str">
         <f aca="false">IF(A56="", "", "L["""&amp;A56&amp;"""] = true")</f>
-        <v>L["Tooltips"] = true</v>
+        <v>L["Clear the permanent ignore list."] = true</v>
       </c>
       <c r="D56" s="1" t="str">
         <f aca="false">IF(A56="", "", "L["""&amp;A56&amp;"""] = """ &amp; B56 &amp; """")</f>
-        <v>L["Tooltips"] = "Mensajes emergentes"</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>L["Clear the permanent ignore list."] = "Limpiar la lista de ignorados permanentemente."</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
         <v>108</v>
       </c>
@@ -1650,11 +1767,11 @@
       </c>
       <c r="C57" s="1" t="str">
         <f aca="false">IF(A57="", "", "L["""&amp;A57&amp;"""] = true")</f>
-        <v>L["Enable tooltips about enchanting materials."] = true</v>
+        <v>L["Uncommon"] = true</v>
       </c>
       <c r="D57" s="1" t="str">
         <f aca="false">IF(A57="", "", "L["""&amp;A57&amp;"""] = """ &amp; B57 &amp; """")</f>
-        <v>L["Enable tooltips about enchanting materials."] = "Activar información sobre materiales de encantamiento."</v>
+        <v>L["Uncommon"] = "Poco Común"</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1666,11 +1783,11 @@
       </c>
       <c r="C58" s="1" t="str">
         <f aca="false">IF(A58="", "", "L["""&amp;A58&amp;"""] = true")</f>
-        <v>L["Database"] = true</v>
+        <v>L["Rare"] = true</v>
       </c>
       <c r="D58" s="1" t="str">
         <f aca="false">IF(A58="", "", "L["""&amp;A58&amp;"""] = """ &amp; B58 &amp; """")</f>
-        <v>L["Database"] = "Base de datos"</v>
+        <v>L["Rare"] = "Raro"</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1682,11 +1799,11 @@
       </c>
       <c r="C59" s="1" t="str">
         <f aca="false">IF(A59="", "", "L["""&amp;A59&amp;"""] = true")</f>
-        <v>L["Update"] = true</v>
+        <v>L["Epic"] = true</v>
       </c>
       <c r="D59" s="1" t="str">
         <f aca="false">IF(A59="", "", "L["""&amp;A59&amp;"""] = """ &amp; B59 &amp; """")</f>
-        <v>L["Update"] = "Actualizar"</v>
+        <v>L["Epic"] = "Epico"</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1698,11 +1815,11 @@
       </c>
       <c r="C60" s="1" t="str">
         <f aca="false">IF(A60="", "", "L["""&amp;A60&amp;"""] = true")</f>
-        <v>L["Update database manually."] = true</v>
+        <v>L["Disable all"] = true</v>
       </c>
       <c r="D60" s="1" t="str">
         <f aca="false">IF(A60="", "", "L["""&amp;A60&amp;"""] = """ &amp; B60 &amp; """")</f>
-        <v>L["Update database manually."] = "Actualizar base de datos manualmente."</v>
+        <v>L["Disable all"] = "Desactivar todo"</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1714,11 +1831,11 @@
       </c>
       <c r="C61" s="1" t="str">
         <f aca="false">IF(A61="", "", "L["""&amp;A61&amp;"""] = true")</f>
-        <v>L["Consolidate"] = true</v>
+        <v>L["Disable all settings."] = true</v>
       </c>
       <c r="D61" s="1" t="str">
         <f aca="false">IF(A61="", "", "L["""&amp;A61&amp;"""] = """ &amp; B61 &amp; """")</f>
-        <v>L["Consolidate"] = "Consolidar"</v>
+        <v>L["Disable all settings."] = "Desactiva todos los ajustes."</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1730,11 +1847,11 @@
       </c>
       <c r="C62" s="1" t="str">
         <f aca="false">IF(A62="", "", "L["""&amp;A62&amp;"""] = true")</f>
-        <v>L["Consolidate players and items in database."] = true</v>
+        <v>L["Tooltips"] = true</v>
       </c>
       <c r="D62" s="1" t="str">
         <f aca="false">IF(A62="", "", "L["""&amp;A62&amp;"""] = """ &amp; B62 &amp; """")</f>
-        <v>L["Consolidate players and items in database."] = "Consolidar jugadores y objetos en la base de datos."</v>
+        <v>L["Tooltips"] = "Mensajes emergentes"</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1746,11 +1863,11 @@
       </c>
       <c r="C63" s="1" t="str">
         <f aca="false">IF(A63="", "", "L["""&amp;A63&amp;"""] = true")</f>
-        <v>L["Are you sure you want to consolidate the database?"] = true</v>
+        <v>L["Enable tooltips about enchanting materials."] = true</v>
       </c>
       <c r="D63" s="1" t="str">
         <f aca="false">IF(A63="", "", "L["""&amp;A63&amp;"""] = """ &amp; B63 &amp; """")</f>
-        <v>L["Are you sure you want to consolidate the database?"] = "¿Estás seguro de que quieres consolidar la base de datos entera?"</v>
+        <v>L["Enable tooltips about enchanting materials."] = "Activar información sobre materiales de encantamiento."</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1758,595 +1875,671 @@
         <v>122</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C64" s="1" t="str">
         <f aca="false">IF(A64="", "", "L["""&amp;A64&amp;"""] = true")</f>
-        <v>L["Clean up"] = true</v>
+        <v>L["Press key to show"] = true</v>
       </c>
       <c r="D64" s="1" t="str">
         <f aca="false">IF(A64="", "", "L["""&amp;A64&amp;"""] = """ &amp; B64 &amp; """")</f>
-        <v>L["Clean up"] = "Limpiar"</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>L["Press key to show"] = "Pulse la tecla para mostrar"</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C65" s="1" t="str">
         <f aca="false">IF(A65="", "", "L["""&amp;A65&amp;"""] = true")</f>
-        <v>L["Clean up all database by removing old data."] = true</v>
+        <v>L["Show title"] = true</v>
       </c>
       <c r="D65" s="1" t="str">
         <f aca="false">IF(A65="", "", "L["""&amp;A65&amp;"""] = """ &amp; B65 &amp; """")</f>
-        <v>L["Clean up all database by removing old data."] = "Limpia toda la base de datos eliminando los datos antiguos."</v>
+        <v>L["Show title"] = "Mostrar título"</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C66" s="1" t="str">
         <f aca="false">IF(A66="", "", "L["""&amp;A66&amp;"""] = true")</f>
-        <v>L["Clean up database"] = true</v>
+        <v>L["Toggle showing title."] = true</v>
       </c>
       <c r="D66" s="1" t="str">
         <f aca="false">IF(A66="", "", "L["""&amp;A66&amp;"""] = """ &amp; B66 &amp; """")</f>
-        <v>L["Clean up database"] = "Limpiar base de datos"</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>L["Toggle showing title."] = "Habilita mostrar el título."</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C67" s="1" t="str">
         <f aca="false">IF(A67="", "", "L["""&amp;A67&amp;"""] = true")</f>
-        <v>L["Are you sure you want to clean up database?"] = true</v>
+        <v>L["Show ItemID"] = true</v>
       </c>
       <c r="D67" s="1" t="str">
         <f aca="false">IF(A67="", "", "L["""&amp;A67&amp;"""] = """ &amp; B67 &amp; """")</f>
-        <v>L["Are you sure you want to clean up database?"] = "¿Estás seguro de que quieres limpiar la base de datos entera?"</v>
+        <v>L["Show ItemID"] = "Mostrar ItemID"</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C68" s="1" t="str">
         <f aca="false">IF(A68="", "", "L["""&amp;A68&amp;"""] = true")</f>
-        <v>L["Purge"] = true</v>
+        <v>L["Toggle showing item ids."] = true</v>
       </c>
       <c r="D68" s="1" t="str">
         <f aca="false">IF(A68="", "", "L["""&amp;A68&amp;"""] = """ &amp; B68 &amp; """")</f>
-        <v>L["Purge"] = "Purgar"</v>
+        <v>L["Toggle showing item ids."] = "Habilita mostrar el ID de objetos."</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C69" s="1" t="str">
         <f aca="false">IF(A69="", "", "L["""&amp;A69&amp;"""] = true")</f>
-        <v>L["Purge all database entries."] = true</v>
+        <v>L["Show zero values"] = true</v>
       </c>
       <c r="D69" s="1" t="str">
         <f aca="false">IF(A69="", "", "L["""&amp;A69&amp;"""] = """ &amp; B69 &amp; """")</f>
-        <v>L["Purge all database entries."] = "Purgar todas las entradas de la base de datos."</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>L["Show zero values"] = "Mostrar valores con cero"</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C70" s="1" t="str">
         <f aca="false">IF(A70="", "", "L["""&amp;A70&amp;"""] = true")</f>
-        <v>L["Are you sure you want to purge entire database?"] = true</v>
+        <v>L["Toggle showing zero values."] = true</v>
       </c>
       <c r="D70" s="1" t="str">
         <f aca="false">IF(A70="", "", "L["""&amp;A70&amp;"""] = """ &amp; B70 &amp; """")</f>
-        <v>L["Are you sure you want to purge entire database?"] = "¿Estás seguro de que quieres purgar la base de datos entera?"</v>
+        <v>L["Toggle showing zero values."] = "Habilita mostrar valores cero."</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C71" s="1" t="str">
         <f aca="false">IF(A71="", "", "L["""&amp;A71&amp;"""] = true")</f>
-        <v>L["Maintenance"] = true</v>
+        <v>L["Items to show"] = true</v>
       </c>
       <c r="D71" s="1" t="str">
         <f aca="false">IF(A71="", "", "L["""&amp;A71&amp;"""] = """ &amp; B71 &amp; """")</f>
-        <v>L["Maintenance"] = "Mantenimiento"</v>
+        <v>L["Items to show"] = "Elementos para mostrar"</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C72" s="1" t="str">
         <f aca="false">IF(A72="", "", "L["""&amp;A72&amp;"""] = true")</f>
-        <v>L["Stats"] = true</v>
+        <v>L["Items to show in tooltip."] = true</v>
       </c>
       <c r="D72" s="1" t="str">
         <f aca="false">IF(A72="", "", "L["""&amp;A72&amp;"""] = """ &amp; B72 &amp; """")</f>
-        <v>L["Stats"] = "Estadísticas"</v>
+        <v>L["Items to show in tooltip."] = "Elementos a mostrar en el mensaje emergente."</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C73" s="1" t="str">
         <f aca="false">IF(A73="", "", "L["""&amp;A73&amp;"""] = true")</f>
-        <v>L["Available commands"] = true</v>
+        <v>L["Show expected essences"] = true</v>
       </c>
       <c r="D73" s="1" t="str">
         <f aca="false">IF(A73="", "", "L["""&amp;A73&amp;"""] = """ &amp; B73 &amp; """")</f>
-        <v>L["Available commands"] = "Comandos disponibles"</v>
+        <v>L["Show expected essences"] = "Mostrar esencias esperadas"</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C74" s="1" t="str">
         <f aca="false">IF(A74="", "", "L["""&amp;A74&amp;"""] = true")</f>
-        <v>L["Auto disenchanting"] = true</v>
+        <v>L["Toggle showing of expected essences on items."] = true</v>
       </c>
       <c r="D74" s="1" t="str">
         <f aca="false">IF(A74="", "", "L["""&amp;A74&amp;"""] = """ &amp; B74 &amp; """")</f>
-        <v>L["Auto disenchanting"] = "Desencantado automático"</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>L["Toggle showing of expected essences on items."] = "Habilita mostrar esencias esperadas en objetos."</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C75" s="1" t="str">
         <f aca="false">IF(A75="", "", "L["""&amp;A75&amp;"""] = true")</f>
-        <v>L["Do not disenchant this item during this game session."] = true</v>
+        <v>L["Show real essences"] = true</v>
       </c>
       <c r="D75" s="1" t="str">
         <f aca="false">IF(A75="", "", "L["""&amp;A75&amp;"""] = """ &amp; B75 &amp; """")</f>
-        <v>L["Do not disenchant this item during this game session."] = "No desencantes este objeto durante esta sesión de juego."</v>
+        <v>L["Show real essences"] = "Mostrar esencias reales"</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C76" s="1" t="str">
         <f aca="false">IF(A76="", "", "L["""&amp;A76&amp;"""] = true")</f>
-        <v>L["No"] = true</v>
+        <v>L["Toggle showing of real essences on items."] = true</v>
       </c>
       <c r="D76" s="1" t="str">
         <f aca="false">IF(A76="", "", "L["""&amp;A76&amp;"""] = """ &amp; B76 &amp; """")</f>
-        <v>L["No"] = "No"</v>
+        <v>L["Toggle showing of real essences on items."] = "Habilita mostrar esencias reales de objetos."</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C77" s="1" t="str">
         <f aca="false">IF(A77="", "", "L["""&amp;A77&amp;"""] = true")</f>
-        <v>L["Proceed with disenchantment."] = true</v>
+        <v>L["Database"] = true</v>
       </c>
       <c r="D77" s="1" t="str">
         <f aca="false">IF(A77="", "", "L["""&amp;A77&amp;"""] = """ &amp; B77 &amp; """")</f>
-        <v>L["Proceed with disenchantment."] = "Proceda con el desencantado."</v>
+        <v>L["Database"] = "Base de datos"</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C78" s="1" t="str">
         <f aca="false">IF(A78="", "", "L["""&amp;A78&amp;"""] = true")</f>
-        <v>L["Yes"] = true</v>
+        <v>L["Update"] = true</v>
       </c>
       <c r="D78" s="1" t="str">
         <f aca="false">IF(A78="", "", "L["""&amp;A78&amp;"""] = """ &amp; B78 &amp; """")</f>
-        <v>L["Yes"] = "Sí"</v>
+        <v>L["Update"] = "Actualizar"</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C79" s="1" t="str">
         <f aca="false">IF(A79="", "", "L["""&amp;A79&amp;"""] = true")</f>
-        <v>L["Add this item to the ignore list."] = true</v>
+        <v>L["Update database manually."] = true</v>
       </c>
       <c r="D79" s="1" t="str">
         <f aca="false">IF(A79="", "", "L["""&amp;A79&amp;"""] = """ &amp; B79 &amp; """")</f>
-        <v>L["Add this item to the ignore list."] = "Añade este elemento a la lista de ignorados."</v>
+        <v>L["Update database manually."] = "Actualizar base de datos manualmente."</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C80" s="1" t="str">
         <f aca="false">IF(A80="", "", "L["""&amp;A80&amp;"""] = true")</f>
-        <v>L["Ignore"] = true</v>
+        <v>L["Consolidate"] = true</v>
       </c>
       <c r="D80" s="1" t="str">
         <f aca="false">IF(A80="", "", "L["""&amp;A80&amp;"""] = """ &amp; B80 &amp; """")</f>
-        <v>L["Ignore"] = "Ignorar"</v>
+        <v>L["Consolidate"] = "Consolidar"</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C81" s="1" t="str">
         <f aca="false">IF(A81="", "", "L["""&amp;A81&amp;"""] = true")</f>
-        <v>L["Close window"] = true</v>
+        <v>L["Consolidate players and items in database."] = true</v>
       </c>
       <c r="D81" s="1" t="str">
         <f aca="false">IF(A81="", "", "L["""&amp;A81&amp;"""] = """ &amp; B81 &amp; """")</f>
-        <v>L["Close window"] = "Cerrar ventana"</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>L["Consolidate players and items in database."] = "Consolidar jugadores y objetos en la base de datos."</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C82" s="1" t="str">
         <f aca="false">IF(A82="", "", "L["""&amp;A82&amp;"""] = true")</f>
-        <v>L["Close"] = true</v>
+        <v>L["Are you sure you want to consolidate the database?"] = true</v>
       </c>
       <c r="D82" s="1" t="str">
         <f aca="false">IF(A82="", "", "L["""&amp;A82&amp;"""] = """ &amp; B82 &amp; """")</f>
-        <v>L["Close"] = "Cerrar"</v>
+        <v>L["Are you sure you want to consolidate the database?"] = "¿Estás seguro de que quieres consolidar la base de datos entera?"</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C83" s="1" t="str">
         <f aca="false">IF(A83="", "", "L["""&amp;A83&amp;"""] = true")</f>
-        <v>L["You don't have enough skill level."] = true</v>
+        <v>L["Clean up"] = true</v>
       </c>
       <c r="D83" s="1" t="str">
         <f aca="false">IF(A83="", "", "L["""&amp;A83&amp;"""] = """ &amp; B83 &amp; """")</f>
-        <v>L["You don't have enough skill level."] = "No tienes suficiente nivel de habilidad."</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>L["Clean up"] = "Limpiar"</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C84" s="1" t="str">
         <f aca="false">IF(A84="", "", "L["""&amp;A84&amp;"""] = true")</f>
-        <v>L["You have enough skill level."] = true</v>
+        <v>L["Clean up all database by removing old data."] = true</v>
       </c>
       <c r="D84" s="1" t="str">
         <f aca="false">IF(A84="", "", "L["""&amp;A84&amp;"""] = """ &amp; B84 &amp; """")</f>
-        <v>L["You have enough skill level."] = "Tienes suficiente nivel de habilidad."</v>
+        <v>L["Clean up all database by removing old data."] = "Limpia toda la base de datos eliminando los datos antiguos."</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C85" s="1" t="str">
         <f aca="false">IF(A85="", "", "L["""&amp;A85&amp;"""] = true")</f>
-        <v>L["Main plugins"] = true</v>
+        <v>L["Clean up database"] = true</v>
       </c>
       <c r="D85" s="1" t="str">
         <f aca="false">IF(A85="", "", "L["""&amp;A85&amp;"""] = """ &amp; B85 &amp; """")</f>
-        <v>L["Main plugins"] = "Plugins principales"</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>L["Clean up database"] = "Limpiar base de datos"</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C86" s="1" t="str">
         <f aca="false">IF(A86="", "", "L["""&amp;A86&amp;"""] = true")</f>
-        <v>L["Settings"] = true</v>
+        <v>L["Are you sure you want to clean up database?"] = true</v>
       </c>
       <c r="D86" s="1" t="str">
         <f aca="false">IF(A86="", "", "L["""&amp;A86&amp;"""] = """ &amp; B86 &amp; """")</f>
-        <v>L["Settings"] = "Configuración"</v>
+        <v>L["Are you sure you want to clean up database?"] = "¿Estás seguro de que quieres limpiar la base de datos entera?"</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="3"/>
-      <c r="B87" s="3"/>
+      <c r="A87" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>169</v>
+      </c>
       <c r="C87" s="1" t="str">
         <f aca="false">IF(A87="", "", "L["""&amp;A87&amp;"""] = true")</f>
-        <v/>
+        <v>L["Purge"] = true</v>
       </c>
       <c r="D87" s="1" t="str">
         <f aca="false">IF(A87="", "", "L["""&amp;A87&amp;"""] = """ &amp; B87 &amp; """")</f>
-        <v/>
+        <v>L["Purge"] = "Purgar"</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="3"/>
-      <c r="B88" s="3"/>
+      <c r="A88" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>171</v>
+      </c>
       <c r="C88" s="1" t="str">
         <f aca="false">IF(A88="", "", "L["""&amp;A88&amp;"""] = true")</f>
-        <v/>
+        <v>L["Purge all database entries."] = true</v>
       </c>
       <c r="D88" s="1" t="str">
         <f aca="false">IF(A88="", "", "L["""&amp;A88&amp;"""] = """ &amp; B88 &amp; """")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="3"/>
-      <c r="B89" s="3"/>
+        <v>L["Purge all database entries."] = "Purgar todas las entradas de la base de datos."</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>173</v>
+      </c>
       <c r="C89" s="1" t="str">
         <f aca="false">IF(A89="", "", "L["""&amp;A89&amp;"""] = true")</f>
-        <v/>
+        <v>L["Are you sure you want to purge entire database?"] = true</v>
       </c>
       <c r="D89" s="1" t="str">
         <f aca="false">IF(A89="", "", "L["""&amp;A89&amp;"""] = """ &amp; B89 &amp; """")</f>
-        <v/>
+        <v>L["Are you sure you want to purge entire database?"] = "¿Estás seguro de que quieres purgar la base de datos entera?"</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="3"/>
-      <c r="B90" s="3"/>
+      <c r="A90" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>175</v>
+      </c>
       <c r="C90" s="1" t="str">
         <f aca="false">IF(A90="", "", "L["""&amp;A90&amp;"""] = true")</f>
-        <v/>
+        <v>L["Maintenance"] = true</v>
       </c>
       <c r="D90" s="1" t="str">
         <f aca="false">IF(A90="", "", "L["""&amp;A90&amp;"""] = """ &amp; B90 &amp; """")</f>
-        <v/>
+        <v>L["Maintenance"] = "Mantenimiento"</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="3"/>
-      <c r="B91" s="3"/>
+      <c r="A91" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>177</v>
+      </c>
       <c r="C91" s="1" t="str">
         <f aca="false">IF(A91="", "", "L["""&amp;A91&amp;"""] = true")</f>
-        <v/>
+        <v>L["Stats"] = true</v>
       </c>
       <c r="D91" s="1" t="str">
         <f aca="false">IF(A91="", "", "L["""&amp;A91&amp;"""] = """ &amp; B91 &amp; """")</f>
-        <v/>
+        <v>L["Stats"] = "Estadísticas"</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="3"/>
-      <c r="B92" s="3"/>
+      <c r="A92" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>179</v>
+      </c>
       <c r="C92" s="1" t="str">
         <f aca="false">IF(A92="", "", "L["""&amp;A92&amp;"""] = true")</f>
-        <v/>
+        <v>L["Available commands"] = true</v>
       </c>
       <c r="D92" s="1" t="str">
         <f aca="false">IF(A92="", "", "L["""&amp;A92&amp;"""] = """ &amp; B92 &amp; """")</f>
-        <v/>
+        <v>L["Available commands"] = "Comandos disponibles"</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="3"/>
-      <c r="B93" s="3"/>
+      <c r="A93" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>181</v>
+      </c>
       <c r="C93" s="1" t="str">
         <f aca="false">IF(A93="", "", "L["""&amp;A93&amp;"""] = true")</f>
-        <v/>
+        <v>L["Auto disenchanting"] = true</v>
       </c>
       <c r="D93" s="1" t="str">
         <f aca="false">IF(A93="", "", "L["""&amp;A93&amp;"""] = """ &amp; B93 &amp; """")</f>
-        <v/>
+        <v>L["Auto disenchanting"] = "Desencantado automático"</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="3"/>
-      <c r="B94" s="3"/>
+      <c r="A94" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>183</v>
+      </c>
       <c r="C94" s="1" t="str">
         <f aca="false">IF(A94="", "", "L["""&amp;A94&amp;"""] = true")</f>
-        <v/>
+        <v>L["Items left"] = true</v>
       </c>
       <c r="D94" s="1" t="str">
         <f aca="false">IF(A94="", "", "L["""&amp;A94&amp;"""] = """ &amp; B94 &amp; """")</f>
-        <v/>
+        <v>L["Items left"] = "Objetos restantes"</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="3"/>
-      <c r="B95" s="3"/>
+      <c r="A95" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>185</v>
+      </c>
       <c r="C95" s="1" t="str">
         <f aca="false">IF(A95="", "", "L["""&amp;A95&amp;"""] = true")</f>
-        <v/>
+        <v>L["Opens settings window."] = true</v>
       </c>
       <c r="D95" s="1" t="str">
         <f aca="false">IF(A95="", "", "L["""&amp;A95&amp;"""] = """ &amp; B95 &amp; """")</f>
-        <v/>
+        <v>L["Opens settings window."] = "Abre la ventana de configuración."</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="3"/>
-      <c r="B96" s="3"/>
+      <c r="A96" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>187</v>
+      </c>
       <c r="C96" s="1" t="str">
         <f aca="false">IF(A96="", "", "L["""&amp;A96&amp;"""] = true")</f>
-        <v/>
+        <v>L["Settings"] = true</v>
       </c>
       <c r="D96" s="1" t="str">
         <f aca="false">IF(A96="", "", "L["""&amp;A96&amp;"""] = """ &amp; B96 &amp; """")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="3"/>
-      <c r="B97" s="3"/>
+        <v>L["Settings"] = "Configuración"</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>189</v>
+      </c>
       <c r="C97" s="1" t="str">
         <f aca="false">IF(A97="", "", "L["""&amp;A97&amp;"""] = true")</f>
-        <v/>
+        <v>L["Do not disenchant this item during this game session."] = true</v>
       </c>
       <c r="D97" s="1" t="str">
         <f aca="false">IF(A97="", "", "L["""&amp;A97&amp;"""] = """ &amp; B97 &amp; """")</f>
-        <v/>
+        <v>L["Do not disenchant this item during this game session."] = "No desencantes este objeto durante esta sesión de juego."</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="3"/>
-      <c r="B98" s="3"/>
+      <c r="A98" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>190</v>
+      </c>
       <c r="C98" s="1" t="str">
         <f aca="false">IF(A98="", "", "L["""&amp;A98&amp;"""] = true")</f>
-        <v/>
+        <v>L["No"] = true</v>
       </c>
       <c r="D98" s="1" t="str">
         <f aca="false">IF(A98="", "", "L["""&amp;A98&amp;"""] = """ &amp; B98 &amp; """")</f>
-        <v/>
+        <v>L["No"] = "No"</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="3"/>
-      <c r="B99" s="3"/>
+      <c r="A99" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>192</v>
+      </c>
       <c r="C99" s="1" t="str">
         <f aca="false">IF(A99="", "", "L["""&amp;A99&amp;"""] = true")</f>
-        <v/>
+        <v>L["Proceed with disenchantment."] = true</v>
       </c>
       <c r="D99" s="1" t="str">
         <f aca="false">IF(A99="", "", "L["""&amp;A99&amp;"""] = """ &amp; B99 &amp; """")</f>
-        <v/>
+        <v>L["Proceed with disenchantment."] = "Proceda con el desencantado."</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="3"/>
-      <c r="B100" s="3"/>
+      <c r="A100" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>194</v>
+      </c>
       <c r="C100" s="1" t="str">
         <f aca="false">IF(A100="", "", "L["""&amp;A100&amp;"""] = true")</f>
-        <v/>
+        <v>L["Yes"] = true</v>
       </c>
       <c r="D100" s="1" t="str">
         <f aca="false">IF(A100="", "", "L["""&amp;A100&amp;"""] = """ &amp; B100 &amp; """")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="3"/>
-      <c r="B101" s="3"/>
+        <v>L["Yes"] = "Sí"</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>196</v>
+      </c>
       <c r="C101" s="1" t="str">
         <f aca="false">IF(A101="", "", "L["""&amp;A101&amp;"""] = true")</f>
-        <v/>
+        <v>L["Add this item to the permanent ignore list."] = true</v>
       </c>
       <c r="D101" s="1" t="str">
         <f aca="false">IF(A101="", "", "L["""&amp;A101&amp;"""] = """ &amp; B101 &amp; """")</f>
-        <v/>
+        <v>L["Add this item to the permanent ignore list."] = "Añade este elemento a la lista de ignorados permanente."</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="3"/>
-      <c r="B102" s="3"/>
+      <c r="A102" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>198</v>
+      </c>
       <c r="C102" s="1" t="str">
         <f aca="false">IF(A102="", "", "L["""&amp;A102&amp;"""] = true")</f>
-        <v/>
+        <v>L["Ignore"] = true</v>
       </c>
       <c r="D102" s="1" t="str">
         <f aca="false">IF(A102="", "", "L["""&amp;A102&amp;"""] = """ &amp; B102 &amp; """")</f>
-        <v/>
+        <v>L["Ignore"] = "Ignorar"</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="3"/>
-      <c r="B103" s="3"/>
+      <c r="A103" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>200</v>
+      </c>
       <c r="C103" s="1" t="str">
         <f aca="false">IF(A103="", "", "L["""&amp;A103&amp;"""] = true")</f>
-        <v/>
+        <v>L["You don't have enough skill level."] = true</v>
       </c>
       <c r="D103" s="1" t="str">
         <f aca="false">IF(A103="", "", "L["""&amp;A103&amp;"""] = """ &amp; B103 &amp; """")</f>
-        <v/>
+        <v>L["You don't have enough skill level."] = "No tienes suficiente nivel de habilidad."</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="3"/>
-      <c r="B104" s="3"/>
+      <c r="A104" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>202</v>
+      </c>
       <c r="C104" s="1" t="str">
         <f aca="false">IF(A104="", "", "L["""&amp;A104&amp;"""] = true")</f>
-        <v/>
+        <v>L["You have enough skill level."] = true</v>
       </c>
       <c r="D104" s="1" t="str">
         <f aca="false">IF(A104="", "", "L["""&amp;A104&amp;"""] = """ &amp; B104 &amp; """")</f>
-        <v/>
+        <v>L["You have enough skill level."] = "Tienes suficiente nivel de habilidad."</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="3"/>
-      <c r="B105" s="3"/>
+      <c r="A105" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>204</v>
+      </c>
       <c r="C105" s="1" t="str">
         <f aca="false">IF(A105="", "", "L["""&amp;A105&amp;"""] = true")</f>
-        <v/>
+        <v>L["Main plugins"] = true</v>
       </c>
       <c r="D105" s="1" t="str">
         <f aca="false">IF(A105="", "", "L["""&amp;A105&amp;"""] = """ &amp; B105 &amp; """")</f>
-        <v/>
+        <v>L["Main plugins"] = "Plugins principales"</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>